<commit_message>
xls missing test case description
update
</commit_message>
<xml_diff>
--- a/TestData/JTPS-DEVQA/ChargeBasisTypes.xlsx
+++ b/TestData/JTPS-DEVQA/ChargeBasisTypes.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="115">
   <si>
     <t>EOF</t>
   </si>
@@ -387,6 +387,12 @@
   </si>
   <si>
     <t>wnd_ChargeBasisTypes</t>
+  </si>
+  <si>
+    <t>TS001</t>
+  </si>
+  <si>
+    <t>ChargeBasisTypes</t>
   </si>
 </sst>
 </file>
@@ -1010,7 +1016,7 @@
   <dimension ref="A1:X73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L11" sqref="L11"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1116,8 +1122,12 @@
       <c r="A2" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="8"/>
+      <c r="B2" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="D2" s="8"/>
       <c r="E2" s="7" t="s">
         <v>7</v>
@@ -1162,8 +1172,12 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="8"/>
+      <c r="B3" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>114</v>
+      </c>
       <c r="D3" s="8"/>
       <c r="E3" s="7" t="s">
         <v>7</v>

</xml_diff>